<commit_message>
Actualización script para no guardar archivos localmente
</commit_message>
<xml_diff>
--- a/formatos/Analisis/asignacion.xlsx
+++ b/formatos/Analisis/asignacion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.valencia\Desktop\Archivos\formatos\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhonny.pineda\Documents\Archivos\Archivos\Formatos\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -654,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CG11316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
@@ -34965,6 +34965,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>